<commit_message>
Allow getting cells from tables in various ways
</commit_message>
<xml_diff>
--- a/example/example.xlsx
+++ b/example/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Blake\Desktop\pyxltab\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD856A35-965D-42EA-BAD1-F40146E7A33D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4260437A-3EB1-4958-823D-BD20B998852D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
   <si>
     <t>Column1</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Table8</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -83,10 +86,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="166" formatCode="0.000000"/>
-    <numFmt numFmtId="167" formatCode="0.00000"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -141,13 +144,13 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -155,6 +158,72 @@
   </cellStyles>
   <dxfs count="39">
     <dxf>
+      <numFmt numFmtId="167" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
       </font>
@@ -164,108 +233,42 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+    </dxf>
+    <dxf>
       <font>
         <i/>
       </font>
-      <numFmt numFmtId="166" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.000000"/>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
     </dxf>
     <dxf>
       <font>
         <b/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -294,13 +297,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD16BABC-487F-4A4C-A81B-E2D8CD210E8D}" name="Table1" displayName="Table1" ref="A2:D7" totalsRowShown="0" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD16BABC-487F-4A4C-A81B-E2D8CD210E8D}" name="Table1" displayName="Table1" ref="A2:D7" totalsRowShown="0" dataDxfId="38">
   <autoFilter ref="A2:D7" xr:uid="{D8A18C1C-9A00-4976-93B5-6BC21A043BBB}"/>
   <tableColumns count="4">
-    <tableColumn id="3" xr3:uid="{F7896117-1DAE-45A7-9745-8834477C5F29}" name="Column1" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{8DAF620B-1E02-46D2-B116-C3564B2EF9A8}" name="Column2" dataDxfId="14"/>
-    <tableColumn id="1" xr3:uid="{CCB271D1-1D09-4513-BDCA-A5F4562DC8C4}" name="Column3" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{488F8C80-5C83-4B6B-8352-3FCCB5B8A594}" name="Column4" dataDxfId="5">
+    <tableColumn id="3" xr3:uid="{F7896117-1DAE-45A7-9745-8834477C5F29}" name="Column1" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{8DAF620B-1E02-46D2-B116-C3564B2EF9A8}" name="Column2" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{CCB271D1-1D09-4513-BDCA-A5F4562DC8C4}" name="Column3" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{488F8C80-5C83-4B6B-8352-3FCCB5B8A594}" name="Column4" dataDxfId="34">
       <calculatedColumnFormula>Table1[[#This Row],[Column2]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -309,98 +312,96 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{658F5B0C-0638-47D0-AAF3-51E8E211BF1F}" name="Table2" displayName="Table2" ref="Y3:AC8" totalsRowShown="0" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{658F5B0C-0638-47D0-AAF3-51E8E211BF1F}" name="Table2" displayName="Table2" ref="Y3:AC8" totalsRowShown="0" dataDxfId="33">
   <autoFilter ref="Y3:AC8" xr:uid="{BFA99555-1A01-4558-8062-F7ADF18A085C}"/>
   <tableColumns count="5">
-    <tableColumn id="3" xr3:uid="{F6031FFC-6B7B-4C0B-8BFA-13FA7F7310F0}" name="Column1" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{D722E458-F106-4209-9246-6AF10159CD53}" name="Column2" dataDxfId="17"/>
-    <tableColumn id="1" xr3:uid="{FD23E7EC-09C4-4AFC-A130-75E4A39FD706}" name="Column3" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{6E971F25-BA9B-4A8E-B80A-AC173F2102DB}" name="Column4" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{578E24C7-FFDA-4F77-8AFC-1E98D6DFE86E}" name="Column5" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{F6031FFC-6B7B-4C0B-8BFA-13FA7F7310F0}" name="Column1" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{D722E458-F106-4209-9246-6AF10159CD53}" name="Column2" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{FD23E7EC-09C4-4AFC-A130-75E4A39FD706}" name="Column3" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{6E971F25-BA9B-4A8E-B80A-AC173F2102DB}" name="Column4" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{578E24C7-FFDA-4F77-8AFC-1E98D6DFE86E}" name="Column5" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{9C8F926C-D06B-4102-85EB-49F362E7EBBA}" name="Table3" displayName="Table3" ref="AA11:AC16" totalsRowShown="0" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{9C8F926C-D06B-4102-85EB-49F362E7EBBA}" name="Table3" displayName="Table3" ref="AA11:AC16" totalsRowShown="0" dataDxfId="27">
   <autoFilter ref="AA11:AC16" xr:uid="{C8FAF92B-D1E2-44BA-848C-1719E7EB9F50}"/>
   <tableColumns count="3">
-    <tableColumn id="3" xr3:uid="{20F39C54-ABA8-47F8-83A7-A5852B86591A}" name="Column1" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{5DB1AABA-6C1B-4644-89AE-FE54B714E99F}" name="Column2" dataDxfId="11"/>
-    <tableColumn id="1" xr3:uid="{E27E6AD7-05E6-4847-9B1C-5899F39D699E}" name="Column3" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{20F39C54-ABA8-47F8-83A7-A5852B86591A}" name="Column1" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{5DB1AABA-6C1B-4644-89AE-FE54B714E99F}" name="Column2" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{E27E6AD7-05E6-4847-9B1C-5899F39D699E}" name="Column3" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D9876472-F7D0-47F2-B46F-C132EEEC9A7A}" name="Table4" displayName="Table4" ref="AC19:AE24" totalsRowShown="0" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D9876472-F7D0-47F2-B46F-C132EEEC9A7A}" name="Table4" displayName="Table4" ref="AC19:AE24" totalsRowShown="0" dataDxfId="23">
   <autoFilter ref="AC19:AE24" xr:uid="{D6AD4F5A-AABB-4097-85F5-18792D225DE4}"/>
   <tableColumns count="3">
-    <tableColumn id="3" xr3:uid="{C98AF497-DDF0-42A7-AC83-AFC19C120989}" name="Column1" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{859FF262-7B30-45D9-9154-F4DF3220AB29}" name="Column2" dataDxfId="1"/>
-    <tableColumn id="1" xr3:uid="{5EA653AF-4EA0-442C-BB61-3B351381D9AF}" name="Column3" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{C98AF497-DDF0-42A7-AC83-AFC19C120989}" name="Column1" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{859FF262-7B30-45D9-9154-F4DF3220AB29}" name="Column2" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{5EA653AF-4EA0-442C-BB61-3B351381D9AF}" name="Column3" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{462BEB78-72F7-42AD-BF02-86B578AD6237}" name="Table5" displayName="Table5" ref="B2:D7" totalsRowShown="0" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{462BEB78-72F7-42AD-BF02-86B578AD6237}" name="Table5" displayName="Table5" ref="B2:D7" totalsRowShown="0" dataDxfId="19">
   <autoFilter ref="B2:D7" xr:uid="{830A867E-E2CC-48C1-A3CE-7C0DA60FA2B8}"/>
   <tableColumns count="3">
-    <tableColumn id="3" xr3:uid="{7ACEC277-8EC8-459B-8645-A26B7B543025}" name="Column1" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{25D8AF78-E3F5-47AE-9F10-020F099B15B9}" name="Column2" dataDxfId="37"/>
-    <tableColumn id="1" xr3:uid="{1ACEEED7-8F69-42D0-B666-0C606C657213}" name="Column3" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{7ACEC277-8EC8-459B-8645-A26B7B543025}" name="Column1" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{25D8AF78-E3F5-47AE-9F10-020F099B15B9}" name="Column2" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{1ACEEED7-8F69-42D0-B666-0C606C657213}" name="Column3" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{B60F7D30-8377-4D39-A411-3E72BBF6B6ED}" name="Table6" displayName="Table6" ref="Q8:S13" totalsRowShown="0" dataDxfId="19">
-  <autoFilter ref="Q8:S13" xr:uid="{76AB36AA-EC72-4BC3-8931-71D4E8CFE5A4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{B60F7D30-8377-4D39-A411-3E72BBF6B6ED}" name="Table6" displayName="Table6" ref="Q8:S14" totalsRowCount="1" dataDxfId="15">
+  <autoFilter ref="Q8:S13" xr:uid="{C6F2DDB6-B420-4BC3-BCD8-16888E340647}"/>
   <tableColumns count="3">
-    <tableColumn id="3" xr3:uid="{77ED0005-2BAA-4EEF-BD12-2FC4173390D0}" name="Column1" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{CB936422-40D5-440D-BDF4-A31048767D30}" name="Column2" dataDxfId="21"/>
-    <tableColumn id="1" xr3:uid="{70E4B018-DF0F-4F5D-A700-EB60EF3374B6}" name="Column3" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{77ED0005-2BAA-4EEF-BD12-2FC4173390D0}" name="Column1" totalsRowLabel="Total" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{CB936422-40D5-440D-BDF4-A31048767D30}" name="Column2" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{70E4B018-DF0F-4F5D-A700-EB60EF3374B6}" name="Column3" totalsRowFunction="sum" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{B4B1672F-079A-4D01-AC62-B2976FC57BEF}" name="Table7" displayName="Table7" ref="W3:Y8" totalsRowShown="0" dataDxfId="31">
-  <autoFilter ref="W3:Y8" xr:uid="{AA2C8D9E-5A31-4550-A125-3F0031A055A1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{B4B1672F-079A-4D01-AC62-B2976FC57BEF}" name="Table7" displayName="Table7" ref="W4:Y8" headerRowCount="0" totalsRowShown="0" dataDxfId="11">
   <tableColumns count="3">
-    <tableColumn id="3" xr3:uid="{DE729CE0-B2FE-43F1-887B-D8E2DE771D94}" name="Column1" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{898903BF-04F0-49F3-A9BC-CEA123B892B5}" name="Column2" dataDxfId="33"/>
-    <tableColumn id="1" xr3:uid="{F714B96A-CA7E-4BC9-8211-BEFF89DE0287}" name="Column3" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{DE729CE0-B2FE-43F1-887B-D8E2DE771D94}" name="Column1" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{898903BF-04F0-49F3-A9BC-CEA123B892B5}" name="Column2" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{F714B96A-CA7E-4BC9-8211-BEFF89DE0287}" name="Column3" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{4BAFA54B-9753-4ED7-AE99-2551A4804DD6}" name="Table8" displayName="Table8" ref="Y26:AA31" totalsRowShown="0" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{4BAFA54B-9753-4ED7-AE99-2551A4804DD6}" name="Table8" displayName="Table8" ref="Y26:AA31" totalsRowShown="0" dataDxfId="7">
   <autoFilter ref="Y26:AA31" xr:uid="{CF2B3421-018D-4361-9844-D1A616D5B003}"/>
   <tableColumns count="3">
-    <tableColumn id="3" xr3:uid="{2EC2250A-21B8-41AF-BA49-D4A34089EDD1}" name="Column1" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{3325FFDB-CA46-48CC-BC59-CE764DEC7058}" name="Column2" dataDxfId="25"/>
-    <tableColumn id="1" xr3:uid="{48AD42CD-A4EE-428D-A9DB-F3EDB2CC71C5}" name="Column3" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{2EC2250A-21B8-41AF-BA49-D4A34089EDD1}" name="Column1" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{3325FFDB-CA46-48CC-BC59-CE764DEC7058}" name="Column2" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{48AD42CD-A4EE-428D-A9DB-F3EDB2CC71C5}" name="Column3" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{5CCBF981-CBC4-43D8-B418-46B1260A6C7C}" name="Table9" displayName="Table9" ref="AB11:AD16" totalsRowShown="0" dataDxfId="27">
-  <autoFilter ref="AB11:AD16" xr:uid="{58775FEC-D3A4-4CEB-A592-CD67DF855161}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{5CCBF981-CBC4-43D8-B418-46B1260A6C7C}" name="Table9" displayName="Table9" ref="AB12:AD17" headerRowCount="0" totalsRowCount="1" dataDxfId="3">
   <tableColumns count="3">
-    <tableColumn id="3" xr3:uid="{DE02A952-A447-4152-9692-942A995D7822}" name="Column1" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{D5839D12-A093-4B9C-88C8-B300C0A69852}" name="Column2" dataDxfId="29"/>
-    <tableColumn id="1" xr3:uid="{10BE923B-FA89-41C8-83AD-767469823372}" name="Column3" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{DE02A952-A447-4152-9692-942A995D7822}" name="Column1" totalsRowLabel="Total" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{D5839D12-A093-4B9C-88C8-B300C0A69852}" name="Column2" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{10BE923B-FA89-41C8-83AD-767469823372}" name="Column3" totalsRowFunction="sum" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -671,7 +672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1027,7 +1028,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D05397B-DBD5-4F36-9288-79EA36C64608}">
   <dimension ref="B1:AD31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1066,15 +1069,6 @@
       <c r="D3" s="5">
         <v>0.9440401850931428</v>
       </c>
-      <c r="W3" t="s">
-        <v>0</v>
-      </c>
-      <c r="X3" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="4" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B4" s="5">
@@ -1214,15 +1208,6 @@
       <c r="S11" s="2">
         <v>0.173748438528875</v>
       </c>
-      <c r="AB11" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="12" spans="2:30" x14ac:dyDescent="0.3">
       <c r="Q12" s="2">
@@ -1265,6 +1250,13 @@
       </c>
     </row>
     <row r="14" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="Q14" t="s">
+        <v>14</v>
+      </c>
+      <c r="S14" s="2">
+        <f>SUBTOTAL(109,Table6[Column3])</f>
+        <v>2.2675294865680815</v>
+      </c>
       <c r="AB14" s="4">
         <v>0.40204977515510365</v>
       </c>
@@ -1297,12 +1289,21 @@
         <v>0.87519319960449127</v>
       </c>
     </row>
-    <row r="25" spans="25:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="25:30" x14ac:dyDescent="0.3">
+      <c r="AB17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD17" s="4">
+        <f>SUBTOTAL(109,Table9[Column3])</f>
+        <v>2.8996330513522013</v>
+      </c>
+    </row>
+    <row r="25" spans="25:30" x14ac:dyDescent="0.3">
       <c r="Y25" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="25:27" x14ac:dyDescent="0.3">
+    <row r="26" spans="25:30" x14ac:dyDescent="0.3">
       <c r="Y26" t="s">
         <v>0</v>
       </c>
@@ -1313,7 +1314,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="25:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="25:30" x14ac:dyDescent="0.3">
       <c r="Y27" s="3">
         <v>5.8734446659182704E-2</v>
       </c>
@@ -1324,7 +1325,7 @@
         <v>0.60153616265294951</v>
       </c>
     </row>
-    <row r="28" spans="25:27" x14ac:dyDescent="0.3">
+    <row r="28" spans="25:30" x14ac:dyDescent="0.3">
       <c r="Y28" s="3">
         <v>0.42355421448181474</v>
       </c>
@@ -1335,7 +1336,7 @@
         <v>0.53883260043781867</v>
       </c>
     </row>
-    <row r="29" spans="25:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="25:30" x14ac:dyDescent="0.3">
       <c r="Y29" s="3">
         <v>0.21900851637129093</v>
       </c>
@@ -1346,7 +1347,7 @@
         <v>0.7726078273282273</v>
       </c>
     </row>
-    <row r="30" spans="25:27" x14ac:dyDescent="0.3">
+    <row r="30" spans="25:30" x14ac:dyDescent="0.3">
       <c r="Y30" s="3">
         <v>0.41417616592676232</v>
       </c>
@@ -1357,7 +1358,7 @@
         <v>0.342074431564795</v>
       </c>
     </row>
-    <row r="31" spans="25:27" x14ac:dyDescent="0.3">
+    <row r="31" spans="25:30" x14ac:dyDescent="0.3">
       <c r="Y31" s="3">
         <v>0.32164429437123199</v>
       </c>

</xml_diff>